<commit_message>
Fixed ide file path issue
</commit_message>
<xml_diff>
--- a/lib/items/WeaponStats.xlsx
+++ b/lib/items/WeaponStats.xlsx
@@ -11,11 +11,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
+  <si>
+    <t>Bad News</t>
+  </si>
   <si>
     <t>Battleaxe</t>
   </si>
   <si>
+    <t>Blunderbuss</t>
+  </si>
+  <si>
     <t>Blowgun</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t>Hand-axe</t>
   </si>
   <si>
+    <t>Hand-Mortar</t>
+  </si>
+  <si>
     <t>Javelin</t>
   </si>
   <si>
@@ -82,12 +91,24 @@
     <t>Morning-star</t>
   </si>
   <si>
+    <t>Musket</t>
+  </si>
+  <si>
     <t>Net</t>
   </si>
   <si>
+    <t>Palm Pistol</t>
+  </si>
+  <si>
+    <t>Pepperbox</t>
+  </si>
+  <si>
     <t>Pike</t>
   </si>
   <si>
+    <t>Pistol</t>
+  </si>
+  <si>
     <t>Quarterstaff</t>
   </si>
   <si>
@@ -124,9 +145,15 @@
     <t>Whip</t>
   </si>
   <si>
+    <t>2d12=P</t>
+  </si>
+  <si>
     <t>1d8=S</t>
   </si>
   <si>
+    <t>2d8=P</t>
+  </si>
+  <si>
     <t>1=P</t>
   </si>
   <si>
@@ -160,6 +187,9 @@
     <t>1d6=S</t>
   </si>
   <si>
+    <t>2d8=F</t>
+  </si>
+  <si>
     <t>1d12=P</t>
   </si>
   <si>
@@ -175,15 +205,21 @@
     <t>1d4=S</t>
   </si>
   <si>
+    <t>true=</t>
+  </si>
+  <si>
     <t>false=</t>
   </si>
   <si>
-    <t>true=</t>
+    <t>Ammunition=Two-handed=Reload 1=Misfire 3=Range (200/800)</t>
   </si>
   <si>
     <t>Versatile(1d10)</t>
   </si>
   <si>
+    <t>Ammunition=Reload 1=Misfire 2=Range (15/60)</t>
+  </si>
+  <si>
     <t>Ammunition=Range (25/100)=Loading</t>
   </si>
   <si>
@@ -217,6 +253,9 @@
     <t>Light=Thrown (20/60)</t>
   </si>
   <si>
+    <t>Ammunition=Reload 1=Misfire 3=Explosive=Ranged (30/600)</t>
+  </si>
+  <si>
     <t>Thrown (30/120)</t>
   </si>
   <si>
@@ -229,7 +268,19 @@
     <t>Ammunition=Range (150/600)=Heavy=Two-Handed</t>
   </si>
   <si>
+    <t>Ammunition=Ranged (120/480)=Two-handed=Reload 1=Misfire 2</t>
+  </si>
+  <si>
     <t>Special=Thrown (5/15)</t>
+  </si>
+  <si>
+    <t>Ammunition=Ranged (40/160)=Light=Reload 1=Misfire 1</t>
+  </si>
+  <si>
+    <t>Ammunition=Ranged (80/320)=Reload 6=Misfire 2</t>
+  </si>
+  <si>
+    <t>Ammunition=Ranged (60/240)=Reload 4=Misfire 1</t>
   </si>
   <si>
     <t>Versatile (1d8)</t>
@@ -619,454 +670,559 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="W2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>53</v>
+      <c r="AR2" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="S5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AM5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>79</v>
+      <c r="AQ5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>